<commit_message>
removing files with salamander sequences. halfway through updating ranitomeya positive control code
</commit_message>
<xml_diff>
--- a/ranitomeya/genome_wide_SWS2_search/output/most_similar_gene_in_nanorana.xlsx
+++ b/ranitomeya/genome_wide_SWS2_search/output/most_similar_gene_in_nanorana.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uricchio/projects/poison/SWS2_code/genome_wide_SWS2_search/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdtarvin/Google_Drive/Documents/Projects/opsins/OPSINS_CODE/ranitomeya/genome_wide_SWS2_search/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0583D27-5811-AB41-BE9C-FAFDD0BEA55B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E24E7EDB-2EE3-084B-B223-154E7B576B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="460" windowWidth="28040" windowHeight="16180"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15740"/>
   </bookViews>
   <sheets>
     <sheet name="most_similar_gene_in_nanorana" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="116">
   <si>
     <t>Mantidactylus_betsileanus_SWS2_SRR5115160</t>
   </si>
@@ -31,22 +31,85 @@
     <t>PREDICTED: Nanorana parkeri blue-sensitive opsin-like (LOC108790454), mRNA</t>
   </si>
   <si>
+    <t>CAJOBX010001114.1_[3.51e-12,_149572,_150466,_0]</t>
+  </si>
+  <si>
+    <t>gi|1072284525|ref|XM_018573067.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri neuropeptide Y receptor type 4-like (LOC108801114), mRNA</t>
+  </si>
+  <si>
     <t>Brachycephalus_pernix_SWS2_DZUP556A38</t>
   </si>
   <si>
+    <t>CAJOBX010006235.1_[2.51e-22,_42452,_42785,_0]</t>
+  </si>
+  <si>
+    <t>gi|1072260864|ref|XM_018560231.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri pinopsin-like (LOC108790053), mRNA</t>
+  </si>
+  <si>
+    <t>CAJOBX010006668.1_[2.85e-11,_23030372,_23031347,_0]</t>
+  </si>
+  <si>
+    <t>gi|1072264038|ref|XM_018561964.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri sphingosine-1-phosphate receptor 1 (S1PR1), mRNA</t>
+  </si>
+  <si>
+    <t>CAJOBX010007180.1_[1.44e-17,_398482,_398764,_0]</t>
+  </si>
+  <si>
+    <t>gi|1072251659|ref|XM_018555250.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri parapinopsin-like (LOC108786042), mRNA</t>
+  </si>
+  <si>
+    <t>CAJOBX010027224.1_[4.15e-15,_257694,_257925,_1]</t>
+  </si>
+  <si>
+    <t>gi|1072277166|ref|XM_018569073.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri opsin-VA-like (LOC108797475), mRNA</t>
+  </si>
+  <si>
     <t>Limnodynastes_peronii_SWS2_SRX5507031</t>
   </si>
   <si>
     <t>Rhinella_spinulosa_SWS2_SRX456145</t>
   </si>
   <si>
+    <t>CAJOBX010007002.1_[2.63e-12,_406137,_406959,_0]</t>
+  </si>
+  <si>
+    <t>gi|1072256178|ref|XM_018557697.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri C-C motif chemokine receptor 6 (CCR6), mRNA</t>
+  </si>
+  <si>
+    <t>CAJOBX010072048.1_[4.38e-19,_15331446,_15331668,_1]</t>
+  </si>
+  <si>
+    <t>gi|1072261797|ref|XM_018560743.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri opsin 1 (cone pigments), short-wave-sensitive (OPN1SW), mRNA</t>
+  </si>
+  <si>
     <t>Iranodon_persicus_SWS2_SRX3347490M</t>
   </si>
   <si>
     <t>Rana_pipiens_SWS2_SRR1185907</t>
   </si>
   <si>
-    <t>C224516402</t>
+    <t>CAJOBX010034670.1_[3.8e-19,_31433,_32369,_1]</t>
   </si>
   <si>
     <t>gi|1072251102|ref|XM_018554953.1|</t>
@@ -55,31 +118,34 @@
     <t>PREDICTED: Nanorana parkeri neuropeptide Y receptor type 2-like (LOC108785804), mRNA</t>
   </si>
   <si>
-    <t>P_RNA_scaffold_13850</t>
-  </si>
-  <si>
-    <t>gi|1072251659|ref|XM_018555250.1|</t>
-  </si>
-  <si>
-    <t>PREDICTED: Nanorana parkeri parapinopsin-like (LOC108786042), mRNA</t>
+    <t>CAJOBX010007180.1_[2.29e-22,_392224,_392560,_0]</t>
   </si>
   <si>
     <t>Centrolene_heloderma_SWS2_SC611</t>
   </si>
   <si>
+    <t>CAJOBX010072048.1_[5.51e-15,_15331997,_15332231,_1]</t>
+  </si>
+  <si>
     <t>Rhinella_marina_SWS2_ONZH01019223</t>
   </si>
   <si>
     <t>Atelopus_ignescens_SWS2_SC5694</t>
   </si>
   <si>
+    <t>CAJOBX010027224.1_[1e-16,_205797,_206043,_1]</t>
+  </si>
+  <si>
     <t>Hyla_cinerea_SWS2_SRR3498302</t>
   </si>
   <si>
     <t>Agalychnis_spurrelli_SWS2_1078</t>
   </si>
   <si>
-    <t>scaffold70671</t>
+    <t>Atelopus_flavescens_SWS2_AF1845</t>
+  </si>
+  <si>
+    <t>CAJOBX010018113.1_[2.29e-21,_1218846,_1219116,_1]</t>
   </si>
   <si>
     <t>gi|1072261745|ref|XM_018560714.1|</t>
@@ -88,7 +154,13 @@
     <t>PREDICTED: Nanorana parkeri opsin 1 (cone pigments), long-wave-sensitive (OPN1LW), mRNA</t>
   </si>
   <si>
-    <t>Atelopus_flavescens_SWS2_AF1845</t>
+    <t>CAJOBX010003901.1_[6e-11,_30860,_31793,_0]</t>
+  </si>
+  <si>
+    <t>gi|1072259916|ref|XM_018559713.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri neuropeptide Y receptor Y2 (NPY2R), mRNA</t>
   </si>
   <si>
     <t>Atelopus_spumarius_SWS2_SC419</t>
@@ -97,13 +169,16 @@
     <t>Osornophryne_antisana_SWS2_SC5957</t>
   </si>
   <si>
-    <t>P_RNA_scaffold_3894</t>
-  </si>
-  <si>
-    <t>gi|1072260864|ref|XM_018560231.1|</t>
-  </si>
-  <si>
-    <t>PREDICTED: Nanorana parkeri pinopsin-like (LOC108790053), mRNA</t>
+    <t>CAJOBX010026903.1_[1.54e-14,_269094,_269271,_1]</t>
+  </si>
+  <si>
+    <t>CAJOBX010072493.1_[9.41e-22,_283690,_284044,_1]</t>
+  </si>
+  <si>
+    <t>gi|1072251612|ref|XM_018555227.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri rhodopsin (RHO), mRNA</t>
   </si>
   <si>
     <t>Pleurodeles_waltl_SWS2_SRX3156544</t>
@@ -112,7 +187,10 @@
     <t>Notophthalmus_viridescens_SWS2_Abdullayevetal2013</t>
   </si>
   <si>
-    <t>P_RNA_scaffold_7323</t>
+    <t>Ambystoma_mexicanum_SWS2_LC180361</t>
+  </si>
+  <si>
+    <t>CAJOBX010013533.1_[1.4e-12,_15655,_15988,_1]</t>
   </si>
   <si>
     <t>gi|1072279157|ref|XM_018570157.1|</t>
@@ -121,16 +199,13 @@
     <t>PREDICTED: Nanorana parkeri parapinopsin-like (LOC108798409), partial mRNA</t>
   </si>
   <si>
-    <t>Ambystoma_mexicanum_SWS2_LC180361</t>
-  </si>
-  <si>
-    <t>scaffold69909</t>
-  </si>
-  <si>
-    <t>gi|1072277166|ref|XM_018569073.1|</t>
-  </si>
-  <si>
-    <t>PREDICTED: Nanorana parkeri opsin-VA-like (LOC108797475), mRNA</t>
+    <t>CAJOBX010026903.1_[5.13e-22,_247160,_247409,_1]</t>
+  </si>
+  <si>
+    <t>CAJOBX010030001.1_[6.98e-15,_8348643,_8349498,_0]</t>
+  </si>
+  <si>
+    <t>CAJOBX010043875.1_[6.82e-15,_4761,_5094,_0]</t>
   </si>
   <si>
     <t>Hynobius_retardatus_SWS2_LE209074</t>
@@ -151,19 +226,16 @@
     <t>Nanorana_parkeri_SWS2_XM0185607131</t>
   </si>
   <si>
-    <t>P_RNA_scaffold_21796</t>
-  </si>
-  <si>
-    <t>scaffold9205</t>
-  </si>
-  <si>
-    <t>gi|1072251612|ref|XM_018555227.1|</t>
-  </si>
-  <si>
-    <t>PREDICTED: Nanorana parkeri rhodopsin (RHO), mRNA</t>
-  </si>
-  <si>
-    <t>scaffold37334</t>
+    <t>CAJOBX010017724.1_[3.01e-14,_94362,_94557,_0]</t>
+  </si>
+  <si>
+    <t>CAJOBX010026903.1_[4.84e-17,_274641,_275001,_1]</t>
+  </si>
+  <si>
+    <t>CAJOBX010017724.1_[1.6e-35,_95096,_95600,_0]</t>
+  </si>
+  <si>
+    <t>CAJOBX010072117.1_[8.99e-14,_9219,_10086,_1]</t>
   </si>
   <si>
     <t>gi|1072265926|ref|XM_018562991.1|</t>
@@ -172,6 +244,12 @@
     <t>PREDICTED: Nanorana parkeri C5a anaphylatoxin chemotactic receptor 1-like (LOC108792253), mRNA</t>
   </si>
   <si>
+    <t>CAJOBX010017724.1_[3.14e-18,_92924,_93353,_0]</t>
+  </si>
+  <si>
+    <t>CAJOBX010072048.1_[2.29e-22,_15332478,_15333183,_1]</t>
+  </si>
+  <si>
     <t>Salamandra_infraimmaculata_SWS2_SRX2775495M</t>
   </si>
   <si>
@@ -196,7 +274,22 @@
     <t>Adenomera_andreae_SWS2_SC6428</t>
   </si>
   <si>
-    <t>scaffold21232</t>
+    <t>CAJOBX010011113.1_[2.12e-12,_13707184,_13708063,_0]</t>
+  </si>
+  <si>
+    <t>gi|1072266844|ref|XM_018563491.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri G protein-coupled receptor 17 (GPR17), mRNA</t>
+  </si>
+  <si>
+    <t>CAJOBX010027224.1_[1.44e-12,_276461,_276830,_1]</t>
+  </si>
+  <si>
+    <t>Xenopus_laevis_SWS2_NM0010891421</t>
+  </si>
+  <si>
+    <t>CAJOBX010007158.1_[1.16e-16,_118592,_118778,_0]</t>
   </si>
   <si>
     <t>gi|1072262086|ref|XM_018560899.1|</t>
@@ -205,34 +298,52 @@
     <t>PREDICTED: Nanorana parkeri pinopsin-like (LOC108790594), mRNA</t>
   </si>
   <si>
-    <t>scaffold13740</t>
-  </si>
-  <si>
-    <t>Xenopus_laevis_SWS2_NM0010891421</t>
-  </si>
-  <si>
-    <t>scaffold86147</t>
+    <t>CAJOBX010072493.1_[2.69e-34,_280471,_280978,_1]</t>
+  </si>
+  <si>
+    <t>CAJOBX010001538.1_[6.5e-15,_21990,_22869,_1]</t>
+  </si>
+  <si>
+    <t>gi|1072279479|ref|XM_018570331.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri somatostatin receptor 2 (SSTR2), mRNA</t>
+  </si>
+  <si>
+    <t>CAJOBX010018668.1_[2.78e-12,_220896,_221478,_0]</t>
+  </si>
+  <si>
+    <t>gi|1072262944|ref|XM_018561364.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri alpha-1A adrenergic receptor-like (LOC108791007), mRNA</t>
   </si>
   <si>
     <t>Atelopus_spurrelli_SWS2_RDT0130</t>
   </si>
   <si>
+    <t>CAJOBX010007158.1_[1.15e-21,_130509,_130746,_0]</t>
+  </si>
+  <si>
     <t>Pyxicephalus_adspersus_SWS2_PZQJ01000014</t>
   </si>
   <si>
+    <t>CAJOBX010007113.1_[1.93e-13,_601816,_602668,_1]</t>
+  </si>
+  <si>
+    <t>gi|1072242458|ref|XM_018566712.1|</t>
+  </si>
+  <si>
+    <t>PREDICTED: Nanorana parkeri somatostatin receptor type 4-like (LOC108795462), mRNA</t>
+  </si>
+  <si>
     <t>Atelopus_glyphus_SWS2_RDT0354</t>
   </si>
   <si>
     <t>Oreolalax_rhodostigmatus_SWS2_SRX3371949</t>
   </si>
   <si>
-    <t>P_RNA_scaffold_3983</t>
-  </si>
-  <si>
-    <t>gi|1072266844|ref|XM_018563491.1|</t>
-  </si>
-  <si>
-    <t>PREDICTED: Nanorana parkeri G protein-coupled receptor 17 (GPR17), mRNA</t>
+    <t>CAJOBX010072427.1_[9.66e-19,_66181,_66439,_1]</t>
   </si>
   <si>
     <t>Scaphiopus_couchii_SWS2_GHBO01125588</t>
@@ -247,19 +358,16 @@
     <t>Brachycephalus_boticario_SWS2_DZUP444</t>
   </si>
   <si>
-    <t>P_RNA_scaffold_20043</t>
+    <t>CAJOBX010072493.1_[5.8e-14,_282063,_282279,_1]</t>
+  </si>
+  <si>
+    <t>CAJOBX010006235.1_[1.21e-11,_50533,_50779,_0]</t>
   </si>
   <si>
     <t>Mantella_baroni_SWS2_LC180362</t>
   </si>
   <si>
-    <t>P_RNA_scaffold_4271</t>
-  </si>
-  <si>
-    <t>gi|1072261797|ref|XM_018560743.1|</t>
-  </si>
-  <si>
-    <t>PREDICTED: Nanorana parkeri opsin 1 (cone pigments), short-wave-sensitive (OPN1SW), mRNA</t>
+    <t>CAJOBX010011392.1_[5.21e-12,_381201,_382035,_0]</t>
   </si>
 </sst>
 </file>
@@ -1101,20 +1209,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.6640625" customWidth="1"/>
+    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1128,7 +1236,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1142,7 +1250,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1156,7 +1264,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1170,7 +1278,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1184,7 +1292,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1198,7 +1306,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -1212,7 +1320,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1226,7 +1334,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -1240,13 +1348,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>2.8300000000000002E-135</v>
+        <v>6.3599999999999999E-108</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -1254,13 +1362,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="C11" s="1">
+        <v>5.3200000000000001E-137</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
@@ -1268,7 +1376,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1282,7 +1390,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1296,609 +1404,917 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.6400000000000001E-89</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>9.9999999999999995E-178</v>
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7.4600000000000001E-121</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.9600000000000002E-70</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.19E-152</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5.35E-95</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
+        <v>103</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.9100000000000001E-163</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C22" s="1">
+        <v>6.9700000000000005E-42</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5.9599999999999999E-40</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.11E-118</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1">
-        <v>7.9400000000000006E-70</v>
+        <v>3.1099999999999999E-67</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4.8499999999999995E-94</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C28" s="1">
-        <v>5.3200000000000001E-137</v>
+        <v>1.34E-41</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="C29" s="1">
+        <v>8.6299999999999999E-68</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2.55E-102</v>
       </c>
       <c r="D30" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="C31" s="1">
+        <v>9.1099999999999994E-71</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3.33E-44</v>
       </c>
       <c r="D32" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
+        <v>97</v>
+      </c>
+      <c r="C33" s="1">
+        <v>4.9899999999999997E-111</v>
       </c>
       <c r="D33" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1.4800000000000001E-89</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1.61E-54</v>
       </c>
       <c r="D35" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1.82E-50</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2.3199999999999999E-68</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C38" s="1">
+        <v>9.9300000000000001E-51</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C39" s="1">
+        <v>4.5499999999999997E-48</v>
       </c>
       <c r="D39" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C40" s="1">
-        <v>6.3599999999999999E-108</v>
+        <v>1.5899999999999999E-159</v>
       </c>
       <c r="D40" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C42" s="1">
-        <v>6.92E-93</v>
+        <v>1.75E-71</v>
       </c>
       <c r="D42" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="C43" s="1">
-        <v>8.2500000000000005E-132</v>
+        <v>5.4600000000000002E-53</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1.6399999999999999E-97</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C45" s="1">
+        <v>6.88E-96</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="C46" s="1">
-        <v>1.1000000000000001E-62</v>
+        <v>4.9099999999999997E-133</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="C47" s="1">
-        <v>3.7599999999999998E-47</v>
+        <v>4.4199999999999999E-51</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C48" s="1">
-        <v>1.9100000000000001E-49</v>
+        <v>4.6E-63</v>
       </c>
       <c r="D48" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C49" s="1">
-        <v>2.7100000000000001E-46</v>
+        <v>1.2600000000000001E-93</v>
       </c>
       <c r="D49" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C50" s="1">
-        <v>7.7600000000000004E-118</v>
+        <v>9.0699999999999992E-62</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1.2000000000000001E-72</v>
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52" s="1">
-        <v>1.1900000000000001E-49</v>
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53" s="1">
-        <v>1.8500000000000001E-43</v>
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>110</v>
       </c>
       <c r="B54" t="s">
-        <v>26</v>
-      </c>
-      <c r="C54" s="1">
-        <v>2.1800000000000001E-69</v>
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="1">
-        <v>5.4599999999999999E-37</v>
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="C56" s="1">
-        <v>6.7799999999999999E-40</v>
+        <v>2.8300000000000002E-135</v>
       </c>
       <c r="D56" t="s">
-        <v>46</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1">
+        <v>7.9400000000000006E-70</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1">
+        <v>9.9999999999999995E-178</v>
+      </c>
+      <c r="D65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>78</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>108</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>88</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D56">
-    <sortCondition ref="D1:D56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D78">
+    <sortCondition ref="A1:A78"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>